<commit_message>
Refactor export logic for billing reports in Excel format
</commit_message>
<xml_diff>
--- a/hospital/domain/service/xlsx/billing_list.xlsx
+++ b/hospital/domain/service/xlsx/billing_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86f1a29df5c25d6e/dev/portfolio/hospital/domain/service/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{B447C9FA-B338-4303-AE59-C0E8A730D5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE60AC3F-8657-4AB0-97A1-BFE68B4EB8C8}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{B447C9FA-B338-4303-AE59-C0E8A730D5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B97E0FA-5074-4F43-B40C-12205FE93908}"/>
   <bookViews>
     <workbookView xWindow="-5112" yWindow="6384" windowWidth="23232" windowHeight="12432" xr2:uid="{D7D51C30-D048-49D5-B51D-5C693F0A75FF}"/>
   </bookViews>
@@ -806,17 +806,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1169,7 +1169,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1249,18 +1249,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B5" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C5" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="27"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
@@ -1270,18 +1261,9 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B6" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C6" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
@@ -1291,18 +1273,9 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B7" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="27"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
@@ -1312,18 +1285,9 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B8" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C8" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="27"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
@@ -1333,39 +1297,21 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B9" s="21" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="21" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="32"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="22" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B10" s="23" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C10" s="23" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="38"/>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -1375,18 +1321,9 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B11" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C11" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="27"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
@@ -1396,18 +1333,9 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B12" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="27"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
@@ -1417,18 +1345,9 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B13" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C13" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="27"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -1438,39 +1357,21 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B14" s="21" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C14" s="21" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="32"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="22" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B15" s="23" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C15" s="23" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="38"/>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
@@ -1480,18 +1381,9 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B16" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C16" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="27"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
@@ -1501,18 +1393,9 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B17" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C17" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="27"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
@@ -1522,18 +1405,9 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C18" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="27"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
@@ -1543,36 +1417,27 @@
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B19" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C19" s="18" t="e">
-        <f xml:space="preserve"> IF(#REF!=0, "",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="33"/>
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="30" t="s">

</xml_diff>